<commit_message>
Data visualization from program
</commit_message>
<xml_diff>
--- a/6014/Homework1/traceroute.xlsx
+++ b/6014/Homework1/traceroute.xlsx
@@ -8,60 +8,77 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epoole/Box Sync/erikpoole/6014/Homework1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EB3ED881-E6B9-8A48-B369-0CE44608D5A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{03E1C3EC-E743-3941-9A0F-88144E42C079}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="15500"/>
+    <workbookView xWindow="1280" yWindow="900" windowWidth="27640" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
+    <sheet name="output_First" sheetId="2" r:id="rId2"/>
+    <sheet name="output_Second" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
-    <t>10.17.128.2</t>
+    <t>208.113.139.241</t>
   </si>
   <si>
-    <t>155.99.130.69</t>
+    <t>Multiple_IP_Addresses</t>
   </si>
   <si>
-    <t>155.99.130.56</t>
+    <t>208.113.156.4</t>
   </si>
   <si>
-    <t>199.104.93.101</t>
+    <t>208.185.23.134</t>
   </si>
   <si>
-    <t>199.104.93.118</t>
+    <t>64.125.31.42</t>
   </si>
   <si>
-    <t>140.197.253.138</t>
+    <t>64.125.30.249</t>
   </si>
   <si>
-    <t>140.197.253.22</t>
+    <t>64.125.29.31</t>
   </si>
   <si>
-    <t>198.71.47.145</t>
+    <t>64.125.29.212</t>
   </si>
   <si>
-    <t>162.252.70.114</t>
+    <t>64.125.29.217</t>
   </si>
   <si>
-    <t>64.57.20.254</t>
+    <t>64.125.30.116</t>
   </si>
   <si>
-    <t>162.252.69.171</t>
+    <t>64.125.31.154</t>
   </si>
   <si>
-    <t>108.170.247.193</t>
+    <t>50.248.116.214</t>
   </si>
   <si>
-    <t>74.125.251.39</t>
+    <t>68.86.83.94</t>
   </si>
   <si>
-    <t>172.217.14.78</t>
+    <t>68.86.84.226</t>
+  </si>
+  <si>
+    <t>68.86.90.225</t>
+  </si>
+  <si>
+    <t>69.139.231.85</t>
+  </si>
+  <si>
+    <t>68.87.171.25</t>
+  </si>
+  <si>
+    <t>96.120.96.157</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
   </si>
 </sst>
 </file>
@@ -642,13 +659,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Router Delay to Youtube.com</a:t>
+              <a:t>Traceroute Time to Cepholofair.com (ms)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -690,6 +702,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Sunday 7:53PM</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -704,101 +719,131 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>output!$A$1:$A$14</c:f>
+              <c:f>output_Second!$A$1:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>10.17.128.2</c:v>
+                  <c:v>10.0.0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155.99.130.69</c:v>
+                  <c:v>96.120.96.157</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>155.99.130.56</c:v>
+                  <c:v>68.87.171.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>199.104.93.101</c:v>
+                  <c:v>69.139.231.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>199.104.93.118</c:v>
+                  <c:v>68.86.90.225</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>140.197.253.138</c:v>
+                  <c:v>68.86.84.226</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140.197.253.22</c:v>
+                  <c:v>68.86.83.94</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>198.71.47.145</c:v>
+                  <c:v>50.248.116.214</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>162.252.70.114</c:v>
+                  <c:v>64.125.31.154</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>64.57.20.254</c:v>
+                  <c:v>64.125.30.116</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>162.252.69.171</c:v>
+                  <c:v>64.125.29.217</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>108.170.247.193</c:v>
+                  <c:v>64.125.29.212</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>74.125.251.39</c:v>
+                  <c:v>64.125.29.31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>172.217.14.78</c:v>
+                  <c:v>64.125.30.249</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64.125.31.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>208.185.23.134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>208.113.156.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Multiple_IP_Addresses</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>208.113.139.241</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$B$1:$B$14</c:f>
+              <c:f>output_First!$B$1:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.4820000000000002</c:v>
+                  <c:v>2.4769999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2146666666699999</c:v>
+                  <c:v>9.1673333333299993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6723333333299999</c:v>
+                  <c:v>10.302</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9630000000000001</c:v>
+                  <c:v>15.177</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3973333333300002</c:v>
+                  <c:v>23.5446666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7596666666699998</c:v>
+                  <c:v>25.645333333300002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1866666666699999</c:v>
+                  <c:v>23.416</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3119999999999998</c:v>
+                  <c:v>22.821666666700001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.949000000000002</c:v>
+                  <c:v>21.323666666699999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.196666666700001</c:v>
+                  <c:v>69.917333333299993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.0756666667</c:v>
+                  <c:v>73.458333333300004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.381666666699999</c:v>
+                  <c:v>69.903666666700005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.845333333299999</c:v>
+                  <c:v>79.597999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.9156666667</c:v>
+                  <c:v>71.536000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>72.101666666699998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.310666666700001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>71.333666666699997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>69.468333333299995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70.950333333299994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -807,6 +852,162 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4CF9-A940-95DA-FA9E75CFC0CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sunday 11:23PM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>output_Second!$A$1:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10.0.0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.120.96.157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.87.171.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.139.231.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.86.90.225</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68.86.84.226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.86.83.94</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50.248.116.214</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.125.31.154</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.125.30.116</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64.125.29.217</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.125.29.212</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64.125.29.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64.125.30.249</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64.125.31.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>208.185.23.134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>208.113.156.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Multiple_IP_Addresses</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>208.113.139.241</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>output_Second!$B$1:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.9530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.074999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.423666666700001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.026666666699999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.285666666699999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.5446666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.0683333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.238333333300002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69.474000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>69.936999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.578999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>77.884666666699999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>68.126666666700004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71.321666666699997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.590666666700002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>69.709000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>69.896333333300007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>68.488666666699999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CF9-A940-95DA-FA9E75CFC0CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -894,7 +1095,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -937,6 +1138,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8476232137649462"/>
+          <c:y val="0.40085611694371537"/>
+          <c:w val="0.14157431709925147"/>
+          <c:h val="0.2100699912510936"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1541,16 +1783,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1875,10 +2117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1886,121 +2128,342 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
-        <v>2.4820000000000002</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2.2146666666699999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.6723333333299999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.9630000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3.3973333333300002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2.7596666666699998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3.1866666666699999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2.3119999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>16.949000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>15.196666666700001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>15.0756666667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>23.381666666699999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>15.845333333299999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <v>14.9156666667</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>2.4769999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>9.1673333333299993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>10.302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>15.177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>23.5446666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>25.645333333300002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>23.416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>22.821666666700001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>21.323666666699999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>69.917333333299993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>73.458333333300004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>69.903666666700005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>79.597999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>71.536000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>72.101666666699998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>70.310666666700001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>71.333666666699997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>69.468333333299995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>70.950333333299994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>1.9530000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>16.074999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>10.423666666700001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>11.208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>23.026666666699999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>22.285666666699999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>22.5446666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>22.0683333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>24.238333333300002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>69.474000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>69.936999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>70.578999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>77.884666666699999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>68.126666666700004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>71.321666666699997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>70.590666666700002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>69.709000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>69.896333333300007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>68.488666666699999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>